<commit_message>
v1.2.0 - see changelog for details
</commit_message>
<xml_diff>
--- a/test/excel/relationship.xlsx
+++ b/test/excel/relationship.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="organisation" sheetId="4" r:id="rId1"/>
+    <sheet name="relationship" sheetId="5" r:id="rId2"/>
+    <sheet name="customer" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>party</t>
   </si>
@@ -72,6 +74,30 @@
   </si>
   <si>
     <t>Acme Ltd</t>
+  </si>
+  <si>
+    <t>dt:startDate</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>wrighty</t>
+  </si>
+  <si>
+    <t>bigTone</t>
+  </si>
+  <si>
+    <t>lee</t>
+  </si>
+  <si>
+    <t>steve</t>
+  </si>
+  <si>
+    <t>sun</t>
+  </si>
+  <si>
+    <t>creditLimit</t>
   </si>
 </sst>
 </file>
@@ -81,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +126,11 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -124,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -136,6 +167,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,4 +640,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>40910</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>40942</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>41004</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>41400</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>41432</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>41463</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>41495</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>41527</v>
+      </c>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>41558</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>41590</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>41609</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>41643</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>41675</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>41702</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>